<commit_message>
added the instructions for testing CSV upload and report generation. Modified the sprint planning and burdown charts to match the commits
</commit_message>
<xml_diff>
--- a/Sprint Backlog/Sprint5 Nov19-26/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
+++ b/Sprint Backlog/Sprint5 Nov19-26/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Sprint Backlog\Sprint5\Planning and Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Sprint Backlog\Sprint5 Nov19-26\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A04153-0868-4792-85A3-695A79F9D155}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D2081-9F13-46F7-8B74-82D5DAE2F240}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>User Stories</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>A:3</t>
+  </si>
+  <si>
+    <t>T24</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1235,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11</c:v>
@@ -2519,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDF196-0978-4E31-AD1C-547BFF446FB7}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,10 +2593,10 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" t="s">
@@ -2617,10 +2620,10 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" t="s">
@@ -2708,7 +2711,9 @@
       <c r="B7" s="4">
         <v>25</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="D7" s="4">
         <v>2</v>
       </c>
@@ -2874,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C753B29C-8070-48CF-BECE-85E4DF604635}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,7 +3012,7 @@
         <v>23</v>
       </c>
       <c r="G5">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>11</v>

</xml_diff>